<commit_message>
docs: clarify variables sheet rules in README
</commit_message>
<xml_diff>
--- a/inst/extdata/AgMIP_protocol/agmip_protocol_vignette.xlsx
+++ b/inst/extdata/AgMIP_protocol/agmip_protocol_vignette.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E9092D-45DB-4883-94B1-A7697312571B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB7CB7F-4C2F-4C55-B644-8D6FF52A1739}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10908" tabRatio="414" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10905" tabRatio="414" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="5" r:id="rId1"/>
@@ -149,180 +149,181 @@
     <t>You can add extra sheets for your own notes or additional information. CroptimizR will only process the recognized sheets (variables, major_parameters, candidate_parameters, fixed_or_computed_parameters) and will ignore any others.</t>
   </si>
   <si>
+    <t>iamfs</t>
+  </si>
+  <si>
+    <t>ilaxs</t>
+  </si>
+  <si>
+    <t>imats</t>
+  </si>
+  <si>
+    <t>masec_n</t>
+  </si>
+  <si>
+    <t>chargefruit</t>
+  </si>
+  <si>
+    <t>mafruit</t>
+  </si>
+  <si>
+    <t>phenology</t>
+  </si>
+  <si>
+    <t>plant_biomass</t>
+  </si>
+  <si>
+    <t>grain_number</t>
+  </si>
+  <si>
+    <t>yield</t>
+  </si>
+  <si>
+    <t>date of amf stage (maximum acceleration of leaf growth, end of juvenile phase), in days after 1st jan of sowing year</t>
+  </si>
+  <si>
+    <t>date of lax stage (leaf index maximum), in days after 1st jan of sowing year</t>
+  </si>
+  <si>
+    <t>date of start of physiological maturity, in days after 1st jan of sowing year</t>
+  </si>
+  <si>
+    <t>biomass of aboveground plant (t.ha-1)</t>
+  </si>
+  <si>
+    <t>number of filling grains or ripe fruits (m-2)</t>
+  </si>
+  <si>
+    <t>biomass of harvested organs (t.ha-1)</t>
+  </si>
+  <si>
+    <t>stlevamf</t>
+  </si>
+  <si>
+    <t>cumulative thermal time between the stages LEV (emergence) and AMF (maximum acceleration of leaf growth, end of juvenile phase) (degree-d)</t>
+  </si>
+  <si>
+    <t>stamflax</t>
+  </si>
+  <si>
+    <t>cumulative thermal time between the stages AMF (maximum acceleration of leaf growth, end of juvenile phase)  and LAX (maximum leaf area index, end of leaf growth )  (degree-d)</t>
+  </si>
+  <si>
+    <t>stdrpmat</t>
+  </si>
+  <si>
+    <t>cumulative thermal time between the stages DRP (starting date of filling of harvested organs) and MAT (maturity)  (degree-d)</t>
+  </si>
+  <si>
+    <t>efcroiveg</t>
+  </si>
+  <si>
+    <t>maximum radiation use efficiency during the vegetative stage (AMF = maximum acceleration of leaf growth, end of juvenile phase - DRP=starting date of filling of harvested) (g.MJ-1 organs)</t>
+  </si>
+  <si>
+    <t>efcroirepro</t>
+  </si>
+  <si>
+    <t>maximum radiation use efficiency during the grain filling phase (DRP= starting date of filling of harvested organs - MAT= maturity), (g.MJ-1)</t>
+  </si>
+  <si>
+    <t>cgrain</t>
+  </si>
+  <si>
+    <t>slope of the relationship between grain number and growth rate (grains.g-1.d)</t>
+  </si>
+  <si>
+    <t>vitircarbT</t>
+  </si>
+  <si>
+    <t>rate of increase of the C harvest index vs thermal time (g grain.g-1.d-1)</t>
+  </si>
+  <si>
+    <t>jvc</t>
+  </si>
+  <si>
+    <t>number of vernalizing days (d)</t>
+  </si>
+  <si>
+    <t>sensrsec</t>
+  </si>
+  <si>
+    <t>index of root sensitivity to drought (1=insensitive) (without dimension)</t>
+  </si>
+  <si>
+    <t>belong</t>
+  </si>
+  <si>
+    <t>parameter of the curve of coleoptile elongation (degree.day-1)</t>
+  </si>
+  <si>
+    <t>jvcmini</t>
+  </si>
+  <si>
+    <t>minimum vernalizing days required (d)</t>
+  </si>
+  <si>
+    <t>stressdev</t>
+  </si>
+  <si>
+    <t>maximum phasic delay allowed due to stresses (without dimension)</t>
+  </si>
+  <si>
+    <t>dlaimaxbrut</t>
+  </si>
+  <si>
+    <t>maximum rate of the setting up of LAI (m2 leaf.plant-1.degree-d-1)</t>
+  </si>
+  <si>
+    <t>durvieF</t>
+  </si>
+  <si>
+    <t>maximal lifespan of an adult leaf expressed in summation of Q10=2 (2**(T-Tbase)) (without dimension)</t>
+  </si>
+  <si>
+    <t>vlaimax</t>
+  </si>
+  <si>
+    <t>ulai at the inflexion point of the function DELTAI=f(ULAI), where ulai is the relative development unit for LAI (without dimension)</t>
+  </si>
+  <si>
+    <t>psisto</t>
+  </si>
+  <si>
+    <t>potential of stomatal closing (absolute value) (bars)</t>
+  </si>
+  <si>
+    <t>psiturg</t>
+  </si>
+  <si>
+    <t>potential of the beginning of decrease of the cellular extension (absolute value) (bars)</t>
+  </si>
+  <si>
+    <t>nbjgrain</t>
+  </si>
+  <si>
+    <t>number of days used to compute the number of viable grains (d)</t>
+  </si>
+  <si>
+    <t>pgrainmaxi</t>
+  </si>
+  <si>
+    <t>maximum grain weight (at 0% water content)</t>
+  </si>
+  <si>
+    <t>cgrainv0</t>
+  </si>
+  <si>
+    <t>fraction of the maximal number of grains when growth rate is zero</t>
+  </si>
+  <si>
+    <t>This Excel file is a fully worked example of an AgMIP calibration protocol, provided to demonstrate the use of CroptimizR in the vignette (adapted from Wallach et al, 2014)</t>
+  </si>
+  <si>
     <t>The order of the groups defines the order of the associated calibration steps in step 6 of the AgMIP protocol.
-Currently, variable names for observed and simulated variables must be identical.
+Group names can be freely chosen by the user.
+At present, the names of observed and simulated variables must be identical and must match the variable names returned by the model wrapper.
 Column description is optional (not used by CroptimizR), the other are required.</t>
-  </si>
-  <si>
-    <t>iamfs</t>
-  </si>
-  <si>
-    <t>ilaxs</t>
-  </si>
-  <si>
-    <t>imats</t>
-  </si>
-  <si>
-    <t>masec_n</t>
-  </si>
-  <si>
-    <t>chargefruit</t>
-  </si>
-  <si>
-    <t>mafruit</t>
-  </si>
-  <si>
-    <t>phenology</t>
-  </si>
-  <si>
-    <t>plant_biomass</t>
-  </si>
-  <si>
-    <t>grain_number</t>
-  </si>
-  <si>
-    <t>yield</t>
-  </si>
-  <si>
-    <t>date of amf stage (maximum acceleration of leaf growth, end of juvenile phase), in days after 1st jan of sowing year</t>
-  </si>
-  <si>
-    <t>date of lax stage (leaf index maximum), in days after 1st jan of sowing year</t>
-  </si>
-  <si>
-    <t>date of start of physiological maturity, in days after 1st jan of sowing year</t>
-  </si>
-  <si>
-    <t>biomass of aboveground plant (t.ha-1)</t>
-  </si>
-  <si>
-    <t>number of filling grains or ripe fruits (m-2)</t>
-  </si>
-  <si>
-    <t>biomass of harvested organs (t.ha-1)</t>
-  </si>
-  <si>
-    <t>stlevamf</t>
-  </si>
-  <si>
-    <t>cumulative thermal time between the stages LEV (emergence) and AMF (maximum acceleration of leaf growth, end of juvenile phase) (degree-d)</t>
-  </si>
-  <si>
-    <t>stamflax</t>
-  </si>
-  <si>
-    <t>cumulative thermal time between the stages AMF (maximum acceleration of leaf growth, end of juvenile phase)  and LAX (maximum leaf area index, end of leaf growth )  (degree-d)</t>
-  </si>
-  <si>
-    <t>stdrpmat</t>
-  </si>
-  <si>
-    <t>cumulative thermal time between the stages DRP (starting date of filling of harvested organs) and MAT (maturity)  (degree-d)</t>
-  </si>
-  <si>
-    <t>efcroiveg</t>
-  </si>
-  <si>
-    <t>maximum radiation use efficiency during the vegetative stage (AMF = maximum acceleration of leaf growth, end of juvenile phase - DRP=starting date of filling of harvested) (g.MJ-1 organs)</t>
-  </si>
-  <si>
-    <t>efcroirepro</t>
-  </si>
-  <si>
-    <t>maximum radiation use efficiency during the grain filling phase (DRP= starting date of filling of harvested organs - MAT= maturity), (g.MJ-1)</t>
-  </si>
-  <si>
-    <t>cgrain</t>
-  </si>
-  <si>
-    <t>slope of the relationship between grain number and growth rate (grains.g-1.d)</t>
-  </si>
-  <si>
-    <t>vitircarbT</t>
-  </si>
-  <si>
-    <t>rate of increase of the C harvest index vs thermal time (g grain.g-1.d-1)</t>
-  </si>
-  <si>
-    <t>jvc</t>
-  </si>
-  <si>
-    <t>number of vernalizing days (d)</t>
-  </si>
-  <si>
-    <t>sensrsec</t>
-  </si>
-  <si>
-    <t>index of root sensitivity to drought (1=insensitive) (without dimension)</t>
-  </si>
-  <si>
-    <t>belong</t>
-  </si>
-  <si>
-    <t>parameter of the curve of coleoptile elongation (degree.day-1)</t>
-  </si>
-  <si>
-    <t>jvcmini</t>
-  </si>
-  <si>
-    <t>minimum vernalizing days required (d)</t>
-  </si>
-  <si>
-    <t>stressdev</t>
-  </si>
-  <si>
-    <t>maximum phasic delay allowed due to stresses (without dimension)</t>
-  </si>
-  <si>
-    <t>dlaimaxbrut</t>
-  </si>
-  <si>
-    <t>maximum rate of the setting up of LAI (m2 leaf.plant-1.degree-d-1)</t>
-  </si>
-  <si>
-    <t>durvieF</t>
-  </si>
-  <si>
-    <t>maximal lifespan of an adult leaf expressed in summation of Q10=2 (2**(T-Tbase)) (without dimension)</t>
-  </si>
-  <si>
-    <t>vlaimax</t>
-  </si>
-  <si>
-    <t>ulai at the inflexion point of the function DELTAI=f(ULAI), where ulai is the relative development unit for LAI (without dimension)</t>
-  </si>
-  <si>
-    <t>psisto</t>
-  </si>
-  <si>
-    <t>potential of stomatal closing (absolute value) (bars)</t>
-  </si>
-  <si>
-    <t>psiturg</t>
-  </si>
-  <si>
-    <t>potential of the beginning of decrease of the cellular extension (absolute value) (bars)</t>
-  </si>
-  <si>
-    <t>nbjgrain</t>
-  </si>
-  <si>
-    <t>number of days used to compute the number of viable grains (d)</t>
-  </si>
-  <si>
-    <t>pgrainmaxi</t>
-  </si>
-  <si>
-    <t>maximum grain weight (at 0% water content)</t>
-  </si>
-  <si>
-    <t>cgrainv0</t>
-  </si>
-  <si>
-    <t>fraction of the maximal number of grains when growth rate is zero</t>
-  </si>
-  <si>
-    <t>This Excel file is a fully worked example of an AgMIP calibration protocol, provided to demonstrate the use of CroptimizR in the vignette (adapted from Wallach et al, 2014)</t>
   </si>
 </sst>
 </file>
@@ -714,48 +715,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDB6BA7A-C37F-4BA0-927B-C76B1690B5C3}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="35.6640625" customWidth="1"/>
-    <col min="4" max="4" width="38.6640625" customWidth="1"/>
-    <col min="6" max="6" width="72.44140625" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" customWidth="1"/>
+    <col min="4" max="4" width="38.7109375" customWidth="1"/>
+    <col min="6" max="6" width="72.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>3</v>
       </c>
@@ -775,7 +776,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>11</v>
       </c>
@@ -792,10 +793,10 @@
         <v>9</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>27</v>
       </c>
@@ -815,7 +816,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>29</v>
       </c>
@@ -835,7 +836,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>31</v>
       </c>
@@ -868,14 +869,14 @@
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.88671875" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="105.5546875" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="105.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -886,70 +887,70 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" t="s">
         <v>48</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>45</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -966,19 +967,19 @@
       <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="78.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="78.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -998,12 +999,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2">
         <v>324.8</v>
@@ -1015,15 +1016,15 @@
         <v>400</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>59</v>
-      </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3">
         <v>446.8</v>
@@ -1035,15 +1036,15 @@
         <v>500</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="B4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="5">
         <v>820</v>
@@ -1055,15 +1056,15 @@
         <v>900</v>
       </c>
       <c r="F4" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>63</v>
-      </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5">
         <v>5.3</v>
@@ -1075,15 +1076,15 @@
         <v>6</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>65</v>
-      </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6">
         <v>3.5</v>
@@ -1095,15 +1096,15 @@
         <v>6</v>
       </c>
       <c r="F6" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>67</v>
-      </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7">
         <v>3.2399999999999998E-2</v>
@@ -1115,15 +1116,15 @@
         <v>0.04</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>69</v>
-      </c>
       <c r="B8" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8">
         <v>3.1E-4</v>
@@ -1135,7 +1136,7 @@
         <v>2E-3</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1152,18 +1153,18 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="73.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="45.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="73.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1183,12 +1184,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2">
         <v>58.363999999999997</v>
@@ -1200,15 +1201,15 @@
         <v>60</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>73</v>
-      </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3">
         <v>0.8</v>
@@ -1220,15 +1221,15 @@
         <v>1</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>75</v>
-      </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4">
         <v>2.2800000000000001E-2</v>
@@ -1240,15 +1241,15 @@
         <v>0.03</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>77</v>
-      </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5">
         <v>11.8</v>
@@ -1260,15 +1261,15 @@
         <v>15</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>79</v>
-      </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6">
         <v>0.6</v>
@@ -1280,15 +1281,15 @@
         <v>1</v>
       </c>
       <c r="F6" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>81</v>
-      </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7">
         <v>3.1879999999999999E-3</v>
@@ -1300,15 +1301,15 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="33" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="31.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>83</v>
-      </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8">
         <v>260</v>
@@ -1320,16 +1321,16 @@
         <v>300</v>
       </c>
       <c r="F8" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:7" ht="33" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
         <v>84</v>
       </c>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="1:7" ht="31.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>85</v>
-      </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9">
         <v>2.38</v>
@@ -1341,16 +1342,16 @@
         <v>2.5</v>
       </c>
       <c r="F9" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
         <v>86</v>
       </c>
-      <c r="G9" s="6"/>
-    </row>
-    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>87</v>
-      </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10">
         <v>12.6</v>
@@ -1362,16 +1363,16 @@
         <v>25</v>
       </c>
       <c r="F10" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="1:7" ht="33" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>88</v>
       </c>
-      <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>89</v>
-      </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11">
         <v>10.6</v>
@@ -1383,16 +1384,16 @@
         <v>15</v>
       </c>
       <c r="F11" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>90</v>
       </c>
-      <c r="G11" s="6"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>91</v>
-      </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C12">
         <v>36</v>
@@ -1404,15 +1405,15 @@
         <v>40</v>
       </c>
       <c r="F12" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>93</v>
-      </c>
       <c r="B13" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C13">
         <v>5.5280000000000003E-2</v>
@@ -1424,15 +1425,15 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="F13" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>95</v>
-      </c>
       <c r="B14" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14">
         <v>4.2000000000000003E-2</v>
@@ -1444,7 +1445,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1457,19 +1458,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB91437-CFEE-439F-BAA5-E4DA36F2B7F7}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42" style="5" customWidth="1"/>
-    <col min="3" max="3" width="65.5546875" customWidth="1"/>
+    <col min="3" max="3" width="65.5703125" customWidth="1"/>
     <col min="4" max="4" width="57" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>2</v>
       </c>
@@ -1484,70 +1485,70 @@
       </c>
       <c r="E1" s="7"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="9"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
       <c r="D3" s="9"/>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="8"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="8"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="8"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="7"/>

</xml_diff>